<commit_message>
Second sheet is populated, and fixed .gitignore
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1124">
   <si>
     <t>AnalyteName</t>
   </si>
@@ -3356,7 +3356,7 @@
     <t>14.248</t>
   </si>
   <si>
-    <t>Analyte 1</t>
+    <t>Analyte 1 (CCL2)</t>
   </si>
   <si>
     <t>GNR1</t>
@@ -3378,6 +3378,15 @@
   </si>
   <si>
     <t>GNR3Signal</t>
+  </si>
+  <si>
+    <t>Analyte 2 (IL-6)</t>
+  </si>
+  <si>
+    <t>Analyte 3 (TNF-a)</t>
+  </si>
+  <si>
+    <t>Analyte 4 (VEGF-A)</t>
   </si>
 </sst>
 </file>
@@ -13058,7 +13067,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13124,6 +13133,500 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:17">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="A15" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="A16" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="A17" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="A18" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="A21" t="s">
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="A22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1115</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1116</v>
+      </c>
+      <c r="F22" t="s">
+        <v>1117</v>
+      </c>
+      <c r="G22" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22" t="s">
+        <v>42</v>
+      </c>
+      <c r="I22" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J22" t="s">
+        <v>1119</v>
+      </c>
+      <c r="K22" t="s">
+        <v>1120</v>
+      </c>
+      <c r="L22" t="s">
+        <v>48</v>
+      </c>
+      <c r="M22" t="s">
+        <v>20</v>
+      </c>
+      <c r="N22" t="s">
+        <v>24</v>
+      </c>
+      <c r="O22" t="s">
+        <v>28</v>
+      </c>
+      <c r="P22" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="A23" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="A25" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="A26" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="A27" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="A29" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="A30" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="A31" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="A32" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
+      <c r="A33" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17">
+      <c r="A34" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17">
+      <c r="A35" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
+      <c r="A36" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17">
+      <c r="A37" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17">
+      <c r="A38" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17">
+      <c r="A41" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17">
+      <c r="A42" t="s">
+        <v>46</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1115</v>
+      </c>
+      <c r="E42" t="s">
+        <v>1116</v>
+      </c>
+      <c r="F42" t="s">
+        <v>1117</v>
+      </c>
+      <c r="G42" t="s">
+        <v>41</v>
+      </c>
+      <c r="H42" t="s">
+        <v>42</v>
+      </c>
+      <c r="I42" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J42" t="s">
+        <v>1119</v>
+      </c>
+      <c r="K42" t="s">
+        <v>1120</v>
+      </c>
+      <c r="L42" t="s">
+        <v>48</v>
+      </c>
+      <c r="M42" t="s">
+        <v>20</v>
+      </c>
+      <c r="N42" t="s">
+        <v>24</v>
+      </c>
+      <c r="O42" t="s">
+        <v>28</v>
+      </c>
+      <c r="P42" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17">
+      <c r="A43" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17">
+      <c r="A44" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17">
+      <c r="A45" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17">
+      <c r="A46" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17">
+      <c r="A47" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17">
+      <c r="A48" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17">
+      <c r="A49" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17">
+      <c r="A50" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17">
+      <c r="A51" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17">
+      <c r="A52" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17">
+      <c r="A53" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17">
+      <c r="A54" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17">
+      <c r="A55" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17">
+      <c r="A56" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17">
+      <c r="A57" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17">
+      <c r="A58" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17">
+      <c r="A61" t="s">
+        <v>1123</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17">
+      <c r="A62" t="s">
+        <v>46</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1114</v>
+      </c>
+      <c r="C62" t="s">
+        <v>1</v>
+      </c>
+      <c r="D62" t="s">
+        <v>1115</v>
+      </c>
+      <c r="E62" t="s">
+        <v>1116</v>
+      </c>
+      <c r="F62" t="s">
+        <v>1117</v>
+      </c>
+      <c r="G62" t="s">
+        <v>41</v>
+      </c>
+      <c r="H62" t="s">
+        <v>42</v>
+      </c>
+      <c r="I62" t="s">
+        <v>1118</v>
+      </c>
+      <c r="J62" t="s">
+        <v>1119</v>
+      </c>
+      <c r="K62" t="s">
+        <v>1120</v>
+      </c>
+      <c r="L62" t="s">
+        <v>48</v>
+      </c>
+      <c r="M62" t="s">
+        <v>20</v>
+      </c>
+      <c r="N62" t="s">
+        <v>24</v>
+      </c>
+      <c r="O62" t="s">
+        <v>28</v>
+      </c>
+      <c r="P62" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17">
+      <c r="A63" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17">
+      <c r="A64" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17">
+      <c r="A65" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17">
+      <c r="A66" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17">
+      <c r="A67" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17">
+      <c r="A68" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17">
+      <c r="A69" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17">
+      <c r="A70" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17">
+      <c r="A71" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17">
+      <c r="A72" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17">
+      <c r="A73" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17">
+      <c r="A74" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17">
+      <c r="A75" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17">
+      <c r="A76" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17">
+      <c r="A77" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17">
+      <c r="A78" t="n">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>